<commit_message>
Final flow charts and data dictionary
</commit_message>
<xml_diff>
--- a/Outputs/DataDictionaryv2.xlsx
+++ b/Outputs/DataDictionaryv2.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="357" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209A1ABB-B1F6-49BA-BAD5-29091DE7CC4E}"/>
   <bookViews>
-    <workbookView xWindow="-33960" yWindow="-1125" windowWidth="28800" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
+    <workbookView xWindow="-34515" yWindow="-3300" windowWidth="28785" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change SMI time so that it is time since diagnosis to avoid colinearity with time since prescription
</commit_message>
<xml_diff>
--- a/Outputs/DataDictionaryv2.xlsx
+++ b/Outputs/DataDictionaryv2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uctvnjl_ucl_ac_uk/Documents/Post doc files/Repurposing/Repurposing-CCBs-in-SMI/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="357" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209A1ABB-B1F6-49BA-BAD5-29091DE7CC4E}"/>
+  <xr:revisionPtr revIDLastSave="358" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5AEECB2-D02F-44FC-9400-1E2C8F29CC37}"/>
   <bookViews>
-    <workbookView xWindow="-34515" yWindow="-3300" windowWidth="28785" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
+    <workbookView minimized="1" xWindow="-36540" yWindow="-2295" windowWidth="28800" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>Antipsychotic at index which is at therapeutic dose</t>
   </si>
   <si>
-    <t>index - SMIEv</t>
-  </si>
-  <si>
     <t>index - FirstPsychDate</t>
   </si>
   <si>
@@ -890,6 +887,9 @@
   </si>
   <si>
     <t>TimeSinceAnyHyp</t>
+  </si>
+  <si>
+    <t>index - diagnosis_date</t>
   </si>
 </sst>
 </file>
@@ -1757,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD21BADF-563A-40CF-A565-6F05AE59398E}">
   <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,16 +1771,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,7 +1903,7 @@
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
         <v>97</v>
@@ -2004,7 +2004,7 @@
         <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,7 +2018,7 @@
         <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,10 +2029,10 @@
         <v>80</v>
       </c>
       <c r="C19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" t="s">
         <v>224</v>
-      </c>
-      <c r="D19" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,10 +2057,10 @@
         <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,13 +2068,13 @@
         <v>143</v>
       </c>
       <c r="B22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" t="s">
         <v>284</v>
       </c>
-      <c r="C22" t="s">
-        <v>285</v>
-      </c>
       <c r="D22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,10 +2236,10 @@
         <v>144</v>
       </c>
       <c r="B34" t="s">
+        <v>285</v>
+      </c>
+      <c r="C34" t="s">
         <v>286</v>
-      </c>
-      <c r="C34" t="s">
-        <v>287</v>
       </c>
       <c r="D34" t="s">
         <v>97</v>
@@ -2278,10 +2278,10 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D42" t="s">
         <v>97</v>
@@ -2362,7 +2362,7 @@
         <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -2418,7 +2418,7 @@
         <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>289</v>
       </c>
       <c r="D47" t="s">
         <v>97</v>
@@ -2432,7 +2432,7 @@
         <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -2446,7 +2446,7 @@
         <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
         <v>97</v>
@@ -2460,7 +2460,7 @@
         <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
         <v>97</v>
@@ -2474,7 +2474,7 @@
         <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
@@ -2488,7 +2488,7 @@
         <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
         <v>97</v>
@@ -2502,7 +2502,7 @@
         <v>90</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
         <v>97</v>
@@ -2516,7 +2516,7 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
         <v>97</v>
@@ -2530,7 +2530,7 @@
         <v>91</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
@@ -2544,7 +2544,7 @@
         <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s">
         <v>97</v>
@@ -2558,7 +2558,7 @@
         <v>86</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s">
         <v>97</v>
@@ -2572,7 +2572,7 @@
         <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
         <v>97</v>
@@ -2586,7 +2586,7 @@
         <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
@@ -2600,7 +2600,7 @@
         <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D60" t="s">
         <v>97</v>
@@ -2614,7 +2614,7 @@
         <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D61" t="s">
         <v>97</v>
@@ -2628,7 +2628,7 @@
         <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D62" t="s">
         <v>97</v>
@@ -2642,7 +2642,7 @@
         <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s">
         <v>97</v>
@@ -2656,10 +2656,10 @@
         <v>38</v>
       </c>
       <c r="C64" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" t="s">
         <v>144</v>
-      </c>
-      <c r="D64" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2670,10 +2670,10 @@
         <v>42</v>
       </c>
       <c r="C65" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" t="s">
         <v>146</v>
-      </c>
-      <c r="D65" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2684,10 +2684,10 @@
         <v>43</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2698,10 +2698,10 @@
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2712,10 +2712,10 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,10 +2726,10 @@
         <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,13 +2737,13 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2751,13 +2751,13 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2765,13 +2765,13 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2779,13 +2779,13 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C73" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2793,13 +2793,13 @@
         <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2807,13 +2807,13 @@
         <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2821,13 +2821,13 @@
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2835,13 +2835,13 @@
         <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2849,13 +2849,13 @@
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D78" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2863,13 +2863,13 @@
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C79" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2877,13 +2877,13 @@
         <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D80" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2891,13 +2891,13 @@
         <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C81" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" t="s">
         <v>237</v>
-      </c>
-      <c r="D81" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2905,13 +2905,13 @@
         <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,13 +2919,13 @@
         <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C83" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D83" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2933,13 +2933,13 @@
         <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C84" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D84" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,13 +2947,13 @@
         <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,13 +2961,13 @@
         <v>138</v>
       </c>
       <c r="B86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D86" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2975,13 +2975,13 @@
         <v>136</v>
       </c>
       <c r="B87" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D87" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2989,13 +2989,13 @@
         <v>134</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3003,13 +3003,13 @@
         <v>132</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C89" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3017,13 +3017,13 @@
         <v>117</v>
       </c>
       <c r="B90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C90" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D90" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3031,13 +3031,13 @@
         <v>118</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C91" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D91" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3045,13 +3045,13 @@
         <v>131</v>
       </c>
       <c r="B92" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C92" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D92" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3059,13 +3059,13 @@
         <v>119</v>
       </c>
       <c r="B93" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3073,13 +3073,13 @@
         <v>120</v>
       </c>
       <c r="B94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D94" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,13 +3087,13 @@
         <v>133</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C95" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D95" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3101,13 +3101,13 @@
         <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C96" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D96" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3115,13 +3115,13 @@
         <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C97" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D97" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3129,13 +3129,13 @@
         <v>135</v>
       </c>
       <c r="B98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C98" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D98" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3143,13 +3143,13 @@
         <v>123</v>
       </c>
       <c r="B99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3157,13 +3157,13 @@
         <v>124</v>
       </c>
       <c r="B100" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C100" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D100" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3171,13 +3171,13 @@
         <v>137</v>
       </c>
       <c r="B101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C101" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D101" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3185,13 +3185,13 @@
         <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C102" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D102" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3199,13 +3199,13 @@
         <v>111</v>
       </c>
       <c r="B103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C103" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D103" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3213,13 +3213,13 @@
         <v>112</v>
       </c>
       <c r="B104" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C104" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D104" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,13 +3227,13 @@
         <v>125</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C105" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D105" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3241,13 +3241,13 @@
         <v>126</v>
       </c>
       <c r="B106" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C106" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D106" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,13 +3255,13 @@
         <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D107" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3269,13 +3269,13 @@
         <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D108" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3283,13 +3283,13 @@
         <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C109" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D109" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3297,13 +3297,13 @@
         <v>140</v>
       </c>
       <c r="B110" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C110" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D110" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3311,13 +3311,13 @@
         <v>129</v>
       </c>
       <c r="B111" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C111" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D111" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3325,13 +3325,13 @@
         <v>130</v>
       </c>
       <c r="B112" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C112" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D112" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3339,13 +3339,13 @@
         <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C113" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D113" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3356,10 +3356,10 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D114" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3370,10 +3370,10 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D115" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3384,10 +3384,10 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3398,10 +3398,10 @@
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D117" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3412,10 +3412,10 @@
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D118" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,10 +3426,10 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3440,10 +3440,10 @@
         <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D120" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3454,10 +3454,10 @@
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D121" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3468,10 +3468,10 @@
         <v>13</v>
       </c>
       <c r="C122" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D122" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3482,10 +3482,10 @@
         <v>14</v>
       </c>
       <c r="C123" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D123" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3496,10 +3496,10 @@
         <v>15</v>
       </c>
       <c r="C124" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3510,10 +3510,10 @@
         <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D125" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3524,10 +3524,10 @@
         <v>17</v>
       </c>
       <c r="C126" t="s">
+        <v>151</v>
+      </c>
+      <c r="D126" t="s">
         <v>152</v>
-      </c>
-      <c r="D126" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3538,10 +3538,10 @@
         <v>18</v>
       </c>
       <c r="C127" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D127" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3552,10 +3552,10 @@
         <v>19</v>
       </c>
       <c r="C128" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,10 +3566,10 @@
         <v>20</v>
       </c>
       <c r="C129" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D129" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3580,10 +3580,10 @@
         <v>21</v>
       </c>
       <c r="C130" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D130" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3594,10 +3594,10 @@
         <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D131" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3608,10 +3608,10 @@
         <v>23</v>
       </c>
       <c r="C132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D132" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3622,10 +3622,10 @@
         <v>24</v>
       </c>
       <c r="C133" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D133" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,10 +3636,10 @@
         <v>25</v>
       </c>
       <c r="C134" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D134" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,10 +3650,10 @@
         <v>51</v>
       </c>
       <c r="C135" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D135" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,10 +3664,10 @@
         <v>52</v>
       </c>
       <c r="C136" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D136" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3678,10 +3678,10 @@
         <v>53</v>
       </c>
       <c r="C137" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D137" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3692,10 +3692,10 @@
         <v>60</v>
       </c>
       <c r="C138" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D138" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3706,10 +3706,10 @@
         <v>62</v>
       </c>
       <c r="C139" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D139" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,13 +3717,13 @@
         <v>80</v>
       </c>
       <c r="B140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C140" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D140" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3731,13 +3731,13 @@
         <v>93</v>
       </c>
       <c r="B141" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C141" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,13 +3745,13 @@
         <v>94</v>
       </c>
       <c r="B142" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D142" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3759,13 +3759,13 @@
         <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C143" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D143" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,10 +3776,10 @@
         <v>35</v>
       </c>
       <c r="C144" t="s">
+        <v>171</v>
+      </c>
+      <c r="D144" t="s">
         <v>172</v>
-      </c>
-      <c r="D144" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3790,10 +3790,10 @@
         <v>36</v>
       </c>
       <c r="C145" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D145" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3804,10 +3804,10 @@
         <v>37</v>
       </c>
       <c r="C146" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D146" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing prior self harm so one is binary and one is count
</commit_message>
<xml_diff>
--- a/Outputs/DataDictionaryv2.xlsx
+++ b/Outputs/DataDictionaryv2.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="358" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5AEECB2-D02F-44FC-9400-1E2C8F29CC37}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-36540" yWindow="-2295" windowWidth="28800" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
+    <workbookView xWindow="-76920" yWindow="-5550" windowWidth="38640" windowHeight="21120" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1434,10 +1434,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1758,7 +1754,7 @@
   <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>